<commit_message>
trabajando en grafica rendimientos
</commit_message>
<xml_diff>
--- a/ArchivosPeergroups/Benchmarks/Historico_ISIMP.xlsx
+++ b/ArchivosPeergroups/Benchmarks/Historico_ISIMP.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="319">
   <si>
     <t>Consula de índices</t>
   </si>
@@ -951,6 +951,18 @@
   </si>
   <si>
     <t>20/03/2025</t>
+  </si>
+  <si>
+    <t>21/03/2025</t>
+  </si>
+  <si>
+    <t>24/03/2025</t>
+  </si>
+  <si>
+    <t>25/03/2025</t>
+  </si>
+  <si>
+    <t>26/03/2025</t>
   </si>
   <si>
     <t>FUENTE: ARYES http://www.aryes.info</t>
@@ -1041,7 +1053,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D312"/>
+  <dimension ref="A1:D316"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5341,14 +5353,70 @@
         <v>8</v>
       </c>
     </row>
+    <row r="309">
+      <c r="A309" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B309" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C309" s="4">
+        <v>292.44955</v>
+      </c>
+      <c r="D309" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B310" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="C310" s="0">
+        <v>292.61495</v>
+      </c>
+      <c r="D310" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="311">
-      <c r="A311" s="5" t="s">
-        <v>313</v>
+      <c r="A311" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B311" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C311" s="4">
+        <v>292.669785</v>
+      </c>
+      <c r="D311" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="312">
-      <c r="A312" s="5" t="s">
-        <v>314</v>
+      <c r="A312" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B312" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="C312" s="0">
+        <v>292.739928</v>
+      </c>
+      <c r="D312" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="5" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="5" t="s">
+        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando exportar a excel
</commit_message>
<xml_diff>
--- a/ArchivosPeergroups/Benchmarks/Historico_ISIMP.xlsx
+++ b/ArchivosPeergroups/Benchmarks/Historico_ISIMP.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="486">
   <si>
     <t>Consula de índices</t>
   </si>
@@ -1461,6 +1461,9 @@
   </si>
   <si>
     <t>23/06/2025</t>
+  </si>
+  <si>
+    <t>24/06/2025</t>
   </si>
   <si>
     <t>FUENTE: ARYES http://www.aryes.info</t>
@@ -1551,7 +1554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D482"/>
+  <dimension ref="A1:D483"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -8231,14 +8234,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="481">
-      <c r="A481" s="5" t="s">
+    <row r="479">
+      <c r="A479" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B479" s="4" t="s">
         <v>483</v>
+      </c>
+      <c r="C479" s="4">
+        <v>298.511093</v>
+      </c>
+      <c r="D479" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="482">
       <c r="A482" s="5" t="s">
         <v>484</v>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" s="5" t="s">
+        <v>485</v>
       </c>
     </row>
   </sheetData>

</xml_diff>